<commit_message>
Actualizar Analisis Excel y Readme
</commit_message>
<xml_diff>
--- a/Análisis Excel/RH_People_Analytics_Análisis_Excel.xlsx
+++ b/Análisis Excel/RH_People_Analytics_Análisis_Excel.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\OneDrive\Documentos\C_Rubis\Master PBi\Repositorio Power Bi\People Analytics Dashboard\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\OneDrive\Documentos\C_Rubis\Master PBi\Repositorio Power Bi\People Analytics Dashboard\Pbip_version\Análisis Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77C1F125-3E88-48B0-9F01-2C2E5527DC6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{872CDDFD-E2EC-4952-999D-EFE1CA93A792}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3079,6 +3079,10 @@
     <xf numFmtId="10" fontId="25" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="32" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="32" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3087,10 +3091,6 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="32" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -25899,7 +25899,7 @@
   <dimension ref="A1:O159"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A105" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q1" activeCellId="1" sqref="D1:D1048576 Q1:Q1048576"/>
       <selection pane="bottomLeft" activeCell="J99" sqref="J99"/>
     </sheetView>
@@ -25920,36 +25920,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="56" t="s">
         <v>371</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
       <c r="M1" s="1"/>
       <c r="O1" s="1"/>
     </row>
     <row r="2" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="58" t="s">
         <v>698</v>
       </c>
-      <c r="B2" s="56"/>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="56"/>
-      <c r="K2" s="56"/>
+      <c r="B2" s="58"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="58"/>
+      <c r="K2" s="58"/>
       <c r="M2" s="1"/>
       <c r="O2" s="1"/>
     </row>
@@ -26468,29 +26468,29 @@
         <f>AVERAGEIFS(BD!$Q:$Q,BD!$L:$L,"Activo")</f>
         <v>3.8690821256038652</v>
       </c>
-      <c r="D58" s="55" t="s">
+      <c r="D58" s="57" t="s">
         <v>712</v>
       </c>
-      <c r="E58" s="55"/>
-      <c r="F58" s="55"/>
-      <c r="G58" s="55"/>
-      <c r="H58" s="55"/>
-      <c r="I58" s="55"/>
-      <c r="J58" s="55"/>
-      <c r="K58" s="55"/>
+      <c r="E58" s="57"/>
+      <c r="F58" s="57"/>
+      <c r="G58" s="57"/>
+      <c r="H58" s="57"/>
+      <c r="I58" s="57"/>
+      <c r="J58" s="57"/>
+      <c r="K58" s="57"/>
     </row>
     <row r="59" spans="1:11" s="13" customFormat="1" ht="15.6" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A59" s="13" t="s">
         <v>697</v>
       </c>
-      <c r="D59" s="55"/>
-      <c r="E59" s="55"/>
-      <c r="F59" s="55"/>
-      <c r="G59" s="55"/>
-      <c r="H59" s="55"/>
-      <c r="I59" s="55"/>
-      <c r="J59" s="55"/>
-      <c r="K59" s="55"/>
+      <c r="D59" s="57"/>
+      <c r="E59" s="57"/>
+      <c r="F59" s="57"/>
+      <c r="G59" s="57"/>
+      <c r="H59" s="57"/>
+      <c r="I59" s="57"/>
+      <c r="J59" s="57"/>
+      <c r="K59" s="57"/>
     </row>
     <row r="60" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.3"/>
     <row r="62" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -26524,19 +26524,19 @@
     </row>
     <row r="83" spans="1:15" outlineLevel="2" x14ac:dyDescent="0.3"/>
     <row r="85" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="56" t="s">
+      <c r="A85" s="58" t="s">
         <v>699</v>
       </c>
-      <c r="B85" s="56"/>
-      <c r="C85" s="56"/>
-      <c r="D85" s="56"/>
-      <c r="E85" s="56"/>
-      <c r="F85" s="56"/>
-      <c r="G85" s="56"/>
-      <c r="H85" s="56"/>
-      <c r="I85" s="56"/>
-      <c r="J85" s="56"/>
-      <c r="K85" s="56"/>
+      <c r="B85" s="58"/>
+      <c r="C85" s="58"/>
+      <c r="D85" s="58"/>
+      <c r="E85" s="58"/>
+      <c r="F85" s="58"/>
+      <c r="G85" s="58"/>
+      <c r="H85" s="58"/>
+      <c r="I85" s="58"/>
+      <c r="J85" s="58"/>
+      <c r="K85" s="58"/>
       <c r="M85" s="1"/>
       <c r="O85" s="1"/>
     </row>
@@ -26645,7 +26645,7 @@
         <v>14</v>
       </c>
       <c r="H99" s="49">
-        <f>G99/$G$106</f>
+        <f t="shared" ref="H99:H105" si="4">G99/$G$106</f>
         <v>0.13592233009708737</v>
       </c>
       <c r="L99" s="16"/>
@@ -26659,7 +26659,7 @@
         <v>31</v>
       </c>
       <c r="D100" s="51">
-        <f t="shared" ref="D100:D105" si="4">C100/$C$106</f>
+        <f t="shared" ref="D100:D105" si="5">C100/$C$106</f>
         <v>0.39240506329113922</v>
       </c>
       <c r="F100" s="18" t="s">
@@ -26670,7 +26670,7 @@
         <v>31</v>
       </c>
       <c r="H100" s="51">
-        <f>G100/$G$106</f>
+        <f t="shared" si="4"/>
         <v>0.30097087378640774</v>
       </c>
       <c r="L100" s="16"/>
@@ -26684,7 +26684,7 @@
         <v>0</v>
       </c>
       <c r="D101" s="49">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F101" s="16" t="s">
@@ -26695,7 +26695,7 @@
         <v>3</v>
       </c>
       <c r="H101" s="49">
-        <f>G101/$G$106</f>
+        <f t="shared" si="4"/>
         <v>2.9126213592233011E-2</v>
       </c>
       <c r="L101" s="16"/>
@@ -26709,7 +26709,7 @@
         <v>40</v>
       </c>
       <c r="D102" s="51">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.50632911392405067</v>
       </c>
       <c r="F102" s="18" t="s">
@@ -26720,7 +26720,7 @@
         <v>40</v>
       </c>
       <c r="H102" s="51">
-        <f>G102/$G$106</f>
+        <f t="shared" si="4"/>
         <v>0.38834951456310679</v>
       </c>
       <c r="L102" s="16"/>
@@ -26734,7 +26734,7 @@
         <v>0</v>
       </c>
       <c r="D103" s="49">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F103" s="16" t="s">
@@ -26745,7 +26745,7 @@
         <v>6</v>
       </c>
       <c r="H103" s="49">
-        <f>G103/$G$106</f>
+        <f t="shared" si="4"/>
         <v>5.8252427184466021E-2</v>
       </c>
     </row>
@@ -26758,7 +26758,7 @@
         <v>8</v>
       </c>
       <c r="D104" s="51">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.10126582278481013</v>
       </c>
       <c r="F104" s="18" t="s">
@@ -26769,7 +26769,7 @@
         <v>8</v>
       </c>
       <c r="H104" s="51">
-        <f>G104/$G$106</f>
+        <f t="shared" si="4"/>
         <v>7.7669902912621352E-2</v>
       </c>
     </row>
@@ -26782,7 +26782,7 @@
         <v>0</v>
       </c>
       <c r="D105" s="49">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F105" s="16" t="s">
@@ -26793,7 +26793,7 @@
         <v>1</v>
       </c>
       <c r="H105" s="49">
-        <f>G105/$G$106</f>
+        <f t="shared" si="4"/>
         <v>9.7087378640776691E-3</v>
       </c>
     </row>
@@ -26898,11 +26898,11 @@
         <v>0</v>
       </c>
       <c r="H114" s="49">
-        <f>G114/$G$121</f>
+        <f t="shared" ref="H114:H120" si="6">G114/$G$121</f>
         <v>0</v>
       </c>
       <c r="I114" s="49">
-        <f>G114/$C$121</f>
+        <f t="shared" ref="I114:I120" si="7">G114/$C$121</f>
         <v>0</v>
       </c>
     </row>
@@ -26916,7 +26916,7 @@
         <v>3</v>
       </c>
       <c r="D115" s="53">
-        <f t="shared" ref="D115:D117" si="5">C115/$C$118</f>
+        <f t="shared" ref="D115:D117" si="8">C115/$C$118</f>
         <v>3.7974683544303799E-2</v>
       </c>
       <c r="F115" s="16" t="s">
@@ -26927,11 +26927,11 @@
         <v>25</v>
       </c>
       <c r="H115" s="49">
-        <f>G115/$G$121</f>
+        <f t="shared" si="6"/>
         <v>0.36231884057971014</v>
       </c>
       <c r="I115" s="49">
-        <f>G115/$C$121</f>
+        <f t="shared" si="7"/>
         <v>0.24271844660194175</v>
       </c>
     </row>
@@ -26945,7 +26945,7 @@
         <v>2</v>
       </c>
       <c r="D116" s="53">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>2.5316455696202531E-2</v>
       </c>
       <c r="F116" s="16" t="s">
@@ -26956,11 +26956,11 @@
         <v>0</v>
       </c>
       <c r="H116" s="49">
-        <f>G116/$G$121</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I116" s="49">
-        <f>G116/$C$121</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -26974,7 +26974,7 @@
         <v>5</v>
       </c>
       <c r="D117" s="53">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>6.3291139240506333E-2</v>
       </c>
       <c r="F117" s="25" t="s">
@@ -26985,11 +26985,11 @@
         <v>37</v>
       </c>
       <c r="H117" s="52">
-        <f>G117/$G$121</f>
+        <f t="shared" si="6"/>
         <v>0.53623188405797106</v>
       </c>
       <c r="I117" s="52">
-        <f>G117/$C$121</f>
+        <f t="shared" si="7"/>
         <v>0.35922330097087379</v>
       </c>
     </row>
@@ -27013,11 +27013,11 @@
         <v>0</v>
       </c>
       <c r="H118" s="49">
-        <f>G118/$G$121</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I118" s="49">
-        <f>G118/$C$121</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -27033,11 +27033,11 @@
         <v>7</v>
       </c>
       <c r="H119" s="49">
-        <f>G119/$G$121</f>
+        <f t="shared" si="6"/>
         <v>0.10144927536231885</v>
       </c>
       <c r="I119" s="49">
-        <f>G119/$C$121</f>
+        <f t="shared" si="7"/>
         <v>6.7961165048543687E-2</v>
       </c>
     </row>
@@ -27051,19 +27051,19 @@
         <v>0</v>
       </c>
       <c r="H120" s="49">
-        <f>G120/$G$121</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I120" s="49">
-        <f>G120/$C$121</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="121" spans="1:9" s="13" customFormat="1" ht="15.6" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B121" s="57" t="s">
+      <c r="B121" s="54" t="s">
         <v>731</v>
       </c>
-      <c r="C121" s="58">
+      <c r="C121" s="55">
         <v>103</v>
       </c>
       <c r="D121" s="33"/>
@@ -27208,7 +27208,7 @@
         <v>5</v>
       </c>
       <c r="D135" s="22">
-        <f t="shared" ref="D135:D136" si="6">C135/$C$137</f>
+        <f t="shared" ref="D135:D136" si="9">C135/$C$137</f>
         <v>0.20833333333333334</v>
       </c>
     </row>
@@ -27221,7 +27221,7 @@
         <v>18</v>
       </c>
       <c r="D136" s="22">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0.75</v>
       </c>
     </row>
@@ -27340,11 +27340,11 @@
         <v>1</v>
       </c>
       <c r="H146" s="27">
-        <f t="shared" ref="H146:H151" si="7">IFERROR(G146/$G$152,0)</f>
+        <f t="shared" ref="H146:H151" si="10">IFERROR(G146/$G$152,0)</f>
         <v>0.16666666666666666</v>
       </c>
       <c r="I146" s="49">
-        <f t="shared" ref="I146:I151" si="8">G146/$C$152</f>
+        <f t="shared" ref="I146:I151" si="11">G146/$C$152</f>
         <v>9.7087378640776691E-3</v>
       </c>
     </row>
@@ -27368,11 +27368,11 @@
         <v>0</v>
       </c>
       <c r="H147" s="22">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I147" s="49">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -27396,11 +27396,11 @@
         <v>5</v>
       </c>
       <c r="H148" s="27">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0.83333333333333337</v>
       </c>
       <c r="I148" s="49">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>4.8543689320388349E-2</v>
       </c>
     </row>
@@ -27413,11 +27413,11 @@
         <v>0</v>
       </c>
       <c r="H149" s="22">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I149" s="49">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -27434,7 +27434,7 @@
         <v>0</v>
       </c>
       <c r="I150" s="49">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -27447,19 +27447,19 @@
         <v>0</v>
       </c>
       <c r="H151" s="22">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I151" s="49">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="152" spans="1:9" s="13" customFormat="1" ht="15.6" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B152" s="57" t="s">
+      <c r="B152" s="54" t="s">
         <v>731</v>
       </c>
-      <c r="C152" s="58">
+      <c r="C152" s="55">
         <v>103</v>
       </c>
       <c r="F152" s="28" t="s">

</xml_diff>